<commit_message>
Update Excel docs with template field mapping and RACI improvements
- Fix cover sheet cell mappings (B3=DocType, C5=Date, C6=Solution, C7=Customer)
- Increase RACI column widths by 30% (8 -> 10)
- Add RACI legend with color-coded explanations
</commit_message>
<xml_diff>
--- a/solution-template/sample-provider/sample-category/sample-solution/delivery/configuration.xlsx
+++ b/solution-template/sample-provider/sample-category/sample-solution/delivery/configuration.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="600" firstSheet="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Cover" sheetId="1" state="visible" r:id="rId1"/>
@@ -21,7 +21,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="16">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -47,12 +47,6 @@
     </font>
     <font>
       <name val="Calibri"/>
-      <color rgb="FF5D6D7E"/>
-      <sz val="11"/>
-      <u val="single"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
       <b val="1"/>
       <color rgb="FFCC0000"/>
       <sz val="12"/>
@@ -71,13 +65,6 @@
       <b val="1"/>
       <color theme="1"/>
       <sz val="12"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <color rgb="FF5D6D7E"/>
-      <sz val="14"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -114,6 +101,13 @@
       <b val="1"/>
       <color rgb="FFCC0000"/>
       <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color rgb="FF5D6D7E"/>
+      <sz val="12"/>
+      <u val="single"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -262,7 +256,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -274,9 +268,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -296,79 +287,79 @@
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="11" fillId="8" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="9" fontId="9" fillId="8" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="5" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="164" fontId="12" fillId="5" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -377,7 +368,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -404,11 +395,13 @@
       <row>11</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="1238250" cy="314325"/>
+    <ext cx="1708214" cy="365379"/>
     <pic>
       <nvPicPr>
         <cNvPr id="2" name="Image 1" descr="Picture"/>
-        <cNvPicPr/>
+        <cNvPicPr>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
+        </cNvPicPr>
       </nvPicPr>
       <blipFill>
         <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
@@ -417,6 +410,10 @@
         </a:stretch>
       </blipFill>
       <spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="209550" y="2032000"/>
+          <a:ext cx="1708214" cy="365379"/>
+        </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
@@ -721,15 +718,15 @@
   </sheetPr>
   <dimension ref="B1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <cols>
     <col width="3" customWidth="1" min="1" max="1"/>
     <col width="25" customWidth="1" min="2" max="2"/>
-    <col width="40" customWidth="1" min="3" max="3"/>
+    <col width="32.81640625" customWidth="1" min="3" max="3"/>
     <col width="3" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
@@ -739,95 +736,89 @@
     </row>
     <row r="2" ht="15" customHeight="1"/>
     <row r="3" ht="40" customHeight="1">
-      <c r="B3" s="16" t="inlineStr">
-        <is>
-          <t>[DOCUMENT TITLE]</t>
-        </is>
-      </c>
-    </row>
-    <row r="4" ht="25" customHeight="1">
-      <c r="B4" s="15" t="inlineStr">
+      <c r="B3" s="33" t="inlineStr">
         <is>
           <t>Configuration Parameters</t>
         </is>
       </c>
     </row>
-    <row r="5" ht="30" customHeight="1">
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Delivery Document</t>
+    <row r="4" ht="18" customHeight="1"/>
+    <row r="5" ht="18" customHeight="1">
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>Generated:</t>
+        </is>
+      </c>
+      <c r="C5" s="3" t="inlineStr">
+        <is>
+          <t>November 27, 2025</t>
         </is>
       </c>
     </row>
     <row r="6" ht="18" customHeight="1">
       <c r="B6" s="2" t="inlineStr">
         <is>
-          <t>Generated:</t>
+          <t>Solution:</t>
         </is>
       </c>
       <c r="C6" s="3" t="inlineStr">
         <is>
-          <t>November 16, 2025</t>
+          <t>Sample Solution</t>
         </is>
       </c>
     </row>
     <row r="7" ht="18" customHeight="1">
       <c r="B7" s="2" t="inlineStr">
         <is>
-          <t>Solution:</t>
+          <t>Customer:</t>
         </is>
       </c>
       <c r="C7" s="3" t="inlineStr">
         <is>
-          <t>November 26, 2025</t>
+          <t>[Customer Name]</t>
         </is>
       </c>
     </row>
     <row r="8" ht="18" customHeight="1">
       <c r="B8" s="2" t="inlineStr">
         <is>
-          <t>Customer:</t>
+          <t>Version:</t>
         </is>
       </c>
       <c r="C8" s="3" t="inlineStr">
         <is>
-          <t>Sample Solution</t>
+          <t>1.0</t>
         </is>
       </c>
     </row>
     <row r="9" ht="18" customHeight="1">
       <c r="B9" s="2" t="inlineStr">
         <is>
-          <t>Version:</t>
-        </is>
-      </c>
-      <c r="C9" s="3" t="inlineStr">
-        <is>
-          <t>[Customer Name]</t>
+          <t>Status:</t>
+        </is>
+      </c>
+      <c r="C9" s="4" t="inlineStr">
+        <is>
+          <t>Draft</t>
         </is>
       </c>
     </row>
     <row r="10" ht="18" customHeight="1">
-      <c r="B10" s="2" t="inlineStr">
-        <is>
-          <t>Status:</t>
-        </is>
-      </c>
-      <c r="C10" s="4" t="inlineStr">
-        <is>
-          <t>Draft</t>
-        </is>
-      </c>
-    </row>
-    <row r="11" ht="40" customHeight="1"/>
+      <c r="B10" s="2" t="n"/>
+      <c r="C10" s="4" t="n"/>
+    </row>
+    <row r="11" ht="18" customHeight="1"/>
     <row r="12" ht="30" customHeight="1">
-      <c r="C12" s="5" t="inlineStr">
+      <c r="C12" s="32" t="inlineStr">
         <is>
           <t>eoframework.org</t>
         </is>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:C3"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
@@ -864,2754 +855,2754 @@
   </cols>
   <sheetData>
     <row r="1" ht="32" customHeight="1">
-      <c r="A1" s="35" t="inlineStr">
+      <c r="A1" s="34" t="inlineStr">
         <is>
           <t>Configuration Parameters</t>
         </is>
       </c>
     </row>
     <row r="2" ht="32" customHeight="1">
-      <c r="A2" s="36" t="inlineStr">
+      <c r="A2" s="35" t="inlineStr">
         <is>
           <t>Parameter Name</t>
         </is>
       </c>
-      <c r="B2" s="36" t="inlineStr">
+      <c r="B2" s="35" t="inlineStr">
         <is>
           <t>Category</t>
         </is>
       </c>
-      <c r="C2" s="36" t="inlineStr">
+      <c r="C2" s="35" t="inlineStr">
         <is>
           <t>Environment</t>
         </is>
       </c>
-      <c r="D2" s="36" t="inlineStr">
+      <c r="D2" s="35" t="inlineStr">
         <is>
           <t>Default Value</t>
         </is>
       </c>
-      <c r="E2" s="36" t="inlineStr">
+      <c r="E2" s="35" t="inlineStr">
         <is>
           <t>Description</t>
         </is>
       </c>
-      <c r="F2" s="36" t="inlineStr">
+      <c r="F2" s="35" t="inlineStr">
         <is>
           <t>Required</t>
         </is>
       </c>
-      <c r="G2" s="36" t="inlineStr">
+      <c r="G2" s="35" t="inlineStr">
         <is>
           <t>Data Type</t>
         </is>
       </c>
-      <c r="H2" s="36" t="inlineStr">
+      <c r="H2" s="35" t="inlineStr">
         <is>
           <t>Validation Rules</t>
         </is>
       </c>
-      <c r="I2" s="36" t="inlineStr">
+      <c r="I2" s="35" t="inlineStr">
         <is>
           <t>Security Level</t>
         </is>
       </c>
-      <c r="J2" s="36" t="inlineStr">
+      <c r="J2" s="35" t="inlineStr">
         <is>
           <t>Owner Team</t>
         </is>
       </c>
-      <c r="K2" s="36" t="inlineStr">
+      <c r="K2" s="35" t="inlineStr">
         <is>
           <t>Dependencies</t>
         </is>
       </c>
-      <c r="L2" s="36" t="inlineStr">
+      <c r="L2" s="35" t="inlineStr">
         <is>
           <t>Notes</t>
         </is>
       </c>
-      <c r="M2" s="36" t="inlineStr">
+      <c r="M2" s="35" t="inlineStr">
         <is>
           <t>Last Updated</t>
         </is>
       </c>
     </row>
     <row r="3" ht="26" customHeight="1">
-      <c r="A3" s="37" t="inlineStr">
+      <c r="A3" s="36" t="inlineStr">
         <is>
           <t>APP_NAME</t>
         </is>
       </c>
-      <c r="B3" s="38" t="inlineStr">
+      <c r="B3" s="37" t="inlineStr">
         <is>
           <t>Application</t>
         </is>
       </c>
-      <c r="C3" s="39" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="D3" s="38" t="inlineStr">
+      <c r="C3" s="38" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="D3" s="37" t="inlineStr">
         <is>
           <t>[Solution Name]</t>
         </is>
       </c>
-      <c r="E3" s="38" t="inlineStr">
+      <c r="E3" s="37" t="inlineStr">
         <is>
           <t>Application identifier for logging and monitoring</t>
         </is>
       </c>
-      <c r="F3" s="39" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G3" s="38" t="inlineStr">
+      <c r="F3" s="38" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G3" s="37" t="inlineStr">
         <is>
           <t>String</t>
         </is>
       </c>
-      <c r="H3" s="38" t="inlineStr">
+      <c r="H3" s="37" t="inlineStr">
         <is>
           <t>Max 50 characters</t>
         </is>
       </c>
-      <c r="I3" s="39" t="inlineStr">
+      <c r="I3" s="38" t="inlineStr">
         <is>
           <t>Public</t>
         </is>
       </c>
-      <c r="J3" s="38" t="inlineStr">
+      <c r="J3" s="37" t="inlineStr">
         <is>
           <t>Development</t>
         </is>
       </c>
-      <c r="K3" s="38" t="inlineStr">
+      <c r="K3" s="37" t="inlineStr">
         <is>
           <t>None</t>
         </is>
       </c>
-      <c r="L3" s="38" t="inlineStr">
+      <c r="L3" s="37" t="inlineStr">
         <is>
           <t>Used in logs and metrics</t>
         </is>
       </c>
-      <c r="M3" s="39" t="inlineStr">
+      <c r="M3" s="38" t="inlineStr">
         <is>
           <t>[DATE]</t>
         </is>
       </c>
     </row>
     <row r="4" ht="26" customHeight="1">
-      <c r="A4" s="40" t="inlineStr">
+      <c r="A4" s="39" t="inlineStr">
         <is>
           <t>APP_VERSION</t>
         </is>
       </c>
-      <c r="B4" s="41" t="inlineStr">
+      <c r="B4" s="40" t="inlineStr">
         <is>
           <t>Application</t>
         </is>
       </c>
-      <c r="C4" s="42" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="D4" s="41" t="inlineStr">
+      <c r="C4" s="41" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="D4" s="40" t="inlineStr">
         <is>
           <t>1.0.0</t>
         </is>
       </c>
-      <c r="E4" s="41" t="inlineStr">
+      <c r="E4" s="40" t="inlineStr">
         <is>
           <t>Current application version</t>
         </is>
       </c>
-      <c r="F4" s="42" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G4" s="41" t="inlineStr">
+      <c r="F4" s="41" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G4" s="40" t="inlineStr">
         <is>
           <t>String</t>
         </is>
       </c>
-      <c r="H4" s="41" t="inlineStr">
+      <c r="H4" s="40" t="inlineStr">
         <is>
           <t>Semantic versioning format</t>
         </is>
       </c>
-      <c r="I4" s="42" t="inlineStr">
+      <c r="I4" s="41" t="inlineStr">
         <is>
           <t>Public</t>
         </is>
       </c>
-      <c r="J4" s="41" t="inlineStr">
+      <c r="J4" s="40" t="inlineStr">
         <is>
           <t>Development</t>
         </is>
       </c>
-      <c r="K4" s="41" t="inlineStr">
+      <c r="K4" s="40" t="inlineStr">
         <is>
           <t>None</t>
         </is>
       </c>
-      <c r="L4" s="41" t="inlineStr">
+      <c r="L4" s="40" t="inlineStr">
         <is>
           <t>Updated with each release</t>
         </is>
       </c>
-      <c r="M4" s="42" t="inlineStr">
+      <c r="M4" s="41" t="inlineStr">
         <is>
           <t>[DATE]</t>
         </is>
       </c>
     </row>
     <row r="5" ht="26" customHeight="1">
-      <c r="A5" s="37" t="inlineStr">
+      <c r="A5" s="36" t="inlineStr">
         <is>
           <t>APP_ENVIRONMENT</t>
         </is>
       </c>
-      <c r="B5" s="38" t="inlineStr">
+      <c r="B5" s="37" t="inlineStr">
         <is>
           <t>Application</t>
         </is>
       </c>
-      <c r="C5" s="39" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="D5" s="38" t="inlineStr">
+      <c r="C5" s="38" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="D5" s="37" t="inlineStr">
         <is>
           <t>development</t>
         </is>
       </c>
-      <c r="E5" s="38" t="inlineStr">
+      <c r="E5" s="37" t="inlineStr">
         <is>
           <t>Deployment environment identifier</t>
         </is>
       </c>
-      <c r="F5" s="39" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G5" s="38" t="inlineStr">
+      <c r="F5" s="38" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G5" s="37" t="inlineStr">
         <is>
           <t>String</t>
         </is>
       </c>
-      <c r="H5" s="38" t="inlineStr">
+      <c r="H5" s="37" t="inlineStr">
         <is>
           <t>development|staging|production</t>
         </is>
       </c>
-      <c r="I5" s="39" t="inlineStr">
+      <c r="I5" s="38" t="inlineStr">
         <is>
           <t>Public</t>
         </is>
       </c>
-      <c r="J5" s="38" t="inlineStr">
+      <c r="J5" s="37" t="inlineStr">
         <is>
           <t>Operations</t>
         </is>
       </c>
-      <c r="K5" s="38" t="inlineStr">
+      <c r="K5" s="37" t="inlineStr">
         <is>
           <t>None</t>
         </is>
       </c>
-      <c r="L5" s="38" t="inlineStr">
+      <c r="L5" s="37" t="inlineStr">
         <is>
           <t>Controls feature flags and logging</t>
         </is>
       </c>
-      <c r="M5" s="39" t="inlineStr">
+      <c r="M5" s="38" t="inlineStr">
         <is>
           <t>[DATE]</t>
         </is>
       </c>
     </row>
     <row r="6" ht="26" customHeight="1">
-      <c r="A6" s="40" t="inlineStr">
+      <c r="A6" s="39" t="inlineStr">
         <is>
           <t>APP_PORT</t>
         </is>
       </c>
-      <c r="B6" s="41" t="inlineStr">
+      <c r="B6" s="40" t="inlineStr">
         <is>
           <t>Application</t>
         </is>
       </c>
-      <c r="C6" s="42" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="D6" s="41" t="inlineStr">
+      <c r="C6" s="41" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="D6" s="40" t="inlineStr">
         <is>
           <t>8080</t>
         </is>
       </c>
-      <c r="E6" s="41" t="inlineStr">
+      <c r="E6" s="40" t="inlineStr">
         <is>
           <t>Port number for application server</t>
         </is>
       </c>
-      <c r="F6" s="42" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G6" s="41" t="inlineStr">
+      <c r="F6" s="41" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G6" s="40" t="inlineStr">
         <is>
           <t>Integer</t>
         </is>
       </c>
-      <c r="H6" s="41" t="inlineStr">
+      <c r="H6" s="40" t="inlineStr">
         <is>
           <t>1024-65535</t>
         </is>
       </c>
-      <c r="I6" s="42" t="inlineStr">
+      <c r="I6" s="41" t="inlineStr">
         <is>
           <t>Public</t>
         </is>
       </c>
-      <c r="J6" s="41" t="inlineStr">
+      <c r="J6" s="40" t="inlineStr">
         <is>
           <t>Infrastructure</t>
         </is>
       </c>
-      <c r="K6" s="41" t="inlineStr">
+      <c r="K6" s="40" t="inlineStr">
         <is>
           <t>Network configuration</t>
         </is>
       </c>
-      <c r="L6" s="41" t="inlineStr">
+      <c r="L6" s="40" t="inlineStr">
         <is>
           <t>Ensure no port conflicts</t>
         </is>
       </c>
-      <c r="M6" s="42" t="inlineStr">
+      <c r="M6" s="41" t="inlineStr">
         <is>
           <t>[DATE]</t>
         </is>
       </c>
     </row>
     <row r="7" ht="26" customHeight="1">
-      <c r="A7" s="37" t="inlineStr">
+      <c r="A7" s="36" t="inlineStr">
         <is>
           <t>APP_LOG_LEVEL</t>
         </is>
       </c>
-      <c r="B7" s="38" t="inlineStr">
+      <c r="B7" s="37" t="inlineStr">
         <is>
           <t>Application</t>
         </is>
       </c>
-      <c r="C7" s="39" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="D7" s="38" t="inlineStr">
+      <c r="C7" s="38" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="D7" s="37" t="inlineStr">
         <is>
           <t>info</t>
         </is>
       </c>
-      <c r="E7" s="38" t="inlineStr">
+      <c r="E7" s="37" t="inlineStr">
         <is>
           <t>Logging verbosity level</t>
         </is>
       </c>
-      <c r="F7" s="39" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G7" s="38" t="inlineStr">
+      <c r="F7" s="38" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G7" s="37" t="inlineStr">
         <is>
           <t>String</t>
         </is>
       </c>
-      <c r="H7" s="38" t="inlineStr">
+      <c r="H7" s="37" t="inlineStr">
         <is>
           <t>debug|info|warn|error</t>
         </is>
       </c>
-      <c r="I7" s="39" t="inlineStr">
+      <c r="I7" s="38" t="inlineStr">
         <is>
           <t>Public</t>
         </is>
       </c>
-      <c r="J7" s="38" t="inlineStr">
+      <c r="J7" s="37" t="inlineStr">
         <is>
           <t>Operations</t>
         </is>
       </c>
-      <c r="K7" s="38" t="inlineStr">
+      <c r="K7" s="37" t="inlineStr">
         <is>
           <t>Monitoring tools</t>
         </is>
       </c>
-      <c r="L7" s="38" t="inlineStr">
+      <c r="L7" s="37" t="inlineStr">
         <is>
           <t>Production should use warn or error</t>
         </is>
       </c>
-      <c r="M7" s="39" t="inlineStr">
+      <c r="M7" s="38" t="inlineStr">
         <is>
           <t>[DATE]</t>
         </is>
       </c>
     </row>
     <row r="8" ht="26" customHeight="1">
-      <c r="A8" s="40" t="inlineStr">
+      <c r="A8" s="39" t="inlineStr">
         <is>
           <t>DB_HOST</t>
         </is>
       </c>
-      <c r="B8" s="41" t="inlineStr">
+      <c r="B8" s="40" t="inlineStr">
         <is>
           <t>Database</t>
         </is>
       </c>
-      <c r="C8" s="42" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="D8" s="41" t="inlineStr">
+      <c r="C8" s="41" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="D8" s="40" t="inlineStr">
         <is>
           <t>[********]</t>
         </is>
       </c>
-      <c r="E8" s="41" t="inlineStr">
+      <c r="E8" s="40" t="inlineStr">
         <is>
           <t>Database server hostname or IP</t>
         </is>
       </c>
-      <c r="F8" s="42" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G8" s="41" t="inlineStr">
+      <c r="F8" s="41" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G8" s="40" t="inlineStr">
         <is>
           <t>String</t>
         </is>
       </c>
-      <c r="H8" s="41" t="inlineStr">
+      <c r="H8" s="40" t="inlineStr">
         <is>
           <t>Valid hostname or IP</t>
         </is>
       </c>
-      <c r="I8" s="42" t="inlineStr">
+      <c r="I8" s="41" t="inlineStr">
         <is>
           <t>Confidential</t>
         </is>
       </c>
-      <c r="J8" s="41" t="inlineStr">
+      <c r="J8" s="40" t="inlineStr">
         <is>
           <t>Database Team</t>
         </is>
       </c>
-      <c r="K8" s="41" t="inlineStr">
+      <c r="K8" s="40" t="inlineStr">
         <is>
           <t>Network connectivity</t>
         </is>
       </c>
-      <c r="L8" s="41" t="inlineStr">
+      <c r="L8" s="40" t="inlineStr">
         <is>
           <t>Use FQDN for production</t>
         </is>
       </c>
-      <c r="M8" s="42" t="inlineStr">
+      <c r="M8" s="41" t="inlineStr">
         <is>
           <t>[DATE]</t>
         </is>
       </c>
     </row>
     <row r="9" ht="26" customHeight="1">
-      <c r="A9" s="37" t="inlineStr">
+      <c r="A9" s="36" t="inlineStr">
         <is>
           <t>DB_PORT</t>
         </is>
       </c>
-      <c r="B9" s="38" t="inlineStr">
+      <c r="B9" s="37" t="inlineStr">
         <is>
           <t>Database</t>
         </is>
       </c>
-      <c r="C9" s="39" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="D9" s="38" t="inlineStr">
+      <c r="C9" s="38" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="D9" s="37" t="inlineStr">
         <is>
           <t>5432</t>
         </is>
       </c>
-      <c r="E9" s="38" t="inlineStr">
+      <c r="E9" s="37" t="inlineStr">
         <is>
           <t>Database server port</t>
         </is>
       </c>
-      <c r="F9" s="39" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G9" s="38" t="inlineStr">
+      <c r="F9" s="38" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G9" s="37" t="inlineStr">
         <is>
           <t>Integer</t>
         </is>
       </c>
-      <c r="H9" s="38" t="inlineStr">
+      <c r="H9" s="37" t="inlineStr">
         <is>
           <t>1-65535</t>
         </is>
       </c>
-      <c r="I9" s="39" t="inlineStr">
+      <c r="I9" s="38" t="inlineStr">
         <is>
           <t>Public</t>
         </is>
       </c>
-      <c r="J9" s="38" t="inlineStr">
+      <c r="J9" s="37" t="inlineStr">
         <is>
           <t>Database Team</t>
         </is>
       </c>
-      <c r="K9" s="38" t="inlineStr">
+      <c r="K9" s="37" t="inlineStr">
         <is>
           <t>Firewall rules</t>
         </is>
       </c>
-      <c r="L9" s="38" t="inlineStr">
+      <c r="L9" s="37" t="inlineStr">
         <is>
           <t>PostgreSQL default port</t>
         </is>
       </c>
-      <c r="M9" s="39" t="inlineStr">
+      <c r="M9" s="38" t="inlineStr">
         <is>
           <t>[DATE]</t>
         </is>
       </c>
     </row>
     <row r="10" ht="26" customHeight="1">
-      <c r="A10" s="40" t="inlineStr">
+      <c r="A10" s="39" t="inlineStr">
         <is>
           <t>DB_NAME</t>
         </is>
       </c>
-      <c r="B10" s="41" t="inlineStr">
+      <c r="B10" s="40" t="inlineStr">
         <is>
           <t>Database</t>
         </is>
       </c>
-      <c r="C10" s="42" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="D10" s="41" t="inlineStr">
+      <c r="C10" s="41" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="D10" s="40" t="inlineStr">
         <is>
           <t>[********]</t>
         </is>
       </c>
-      <c r="E10" s="41" t="inlineStr">
+      <c r="E10" s="40" t="inlineStr">
         <is>
           <t>Database name to connect to</t>
         </is>
       </c>
-      <c r="F10" s="42" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G10" s="41" t="inlineStr">
+      <c r="F10" s="41" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G10" s="40" t="inlineStr">
         <is>
           <t>String</t>
         </is>
       </c>
-      <c r="H10" s="41" t="inlineStr">
+      <c r="H10" s="40" t="inlineStr">
         <is>
           <t>Valid database identifier</t>
         </is>
       </c>
-      <c r="I10" s="42" t="inlineStr">
+      <c r="I10" s="41" t="inlineStr">
         <is>
           <t>Confidential</t>
         </is>
       </c>
-      <c r="J10" s="41" t="inlineStr">
+      <c r="J10" s="40" t="inlineStr">
         <is>
           <t>Database Team</t>
         </is>
       </c>
-      <c r="K10" s="41" t="inlineStr">
+      <c r="K10" s="40" t="inlineStr">
         <is>
           <t>Database creation</t>
         </is>
       </c>
-      <c r="L10" s="41" t="inlineStr">
+      <c r="L10" s="40" t="inlineStr">
         <is>
           <t>Must exist before deployment</t>
         </is>
       </c>
-      <c r="M10" s="42" t="inlineStr">
+      <c r="M10" s="41" t="inlineStr">
         <is>
           <t>[DATE]</t>
         </is>
       </c>
     </row>
     <row r="11" ht="26" customHeight="1">
-      <c r="A11" s="37" t="inlineStr">
+      <c r="A11" s="36" t="inlineStr">
         <is>
           <t>DB_USERNAME</t>
         </is>
       </c>
-      <c r="B11" s="38" t="inlineStr">
+      <c r="B11" s="37" t="inlineStr">
         <is>
           <t>Database</t>
         </is>
       </c>
-      <c r="C11" s="39" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="D11" s="38" t="inlineStr">
+      <c r="C11" s="38" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="D11" s="37" t="inlineStr">
         <is>
           <t>[********]</t>
         </is>
       </c>
-      <c r="E11" s="38" t="inlineStr">
+      <c r="E11" s="37" t="inlineStr">
         <is>
           <t>Database connection username</t>
         </is>
       </c>
-      <c r="F11" s="39" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G11" s="38" t="inlineStr">
+      <c r="F11" s="38" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G11" s="37" t="inlineStr">
         <is>
           <t>String</t>
         </is>
       </c>
-      <c r="H11" s="38" t="inlineStr">
+      <c r="H11" s="37" t="inlineStr">
         <is>
           <t>Valid username format</t>
         </is>
       </c>
-      <c r="I11" s="39" t="inlineStr">
+      <c r="I11" s="38" t="inlineStr">
         <is>
           <t>Secret</t>
         </is>
       </c>
-      <c r="J11" s="38" t="inlineStr">
+      <c r="J11" s="37" t="inlineStr">
         <is>
           <t>Database Team</t>
         </is>
       </c>
-      <c r="K11" s="38" t="inlineStr">
+      <c r="K11" s="37" t="inlineStr">
         <is>
           <t>User creation</t>
         </is>
       </c>
-      <c r="L11" s="38" t="inlineStr">
+      <c r="L11" s="37" t="inlineStr">
         <is>
           <t>Use service account</t>
         </is>
       </c>
-      <c r="M11" s="39" t="inlineStr">
+      <c r="M11" s="38" t="inlineStr">
         <is>
           <t>[DATE]</t>
         </is>
       </c>
     </row>
     <row r="12" ht="26" customHeight="1">
-      <c r="A12" s="40" t="inlineStr">
+      <c r="A12" s="39" t="inlineStr">
         <is>
           <t>DB_PASSWORD</t>
         </is>
       </c>
-      <c r="B12" s="41" t="inlineStr">
+      <c r="B12" s="40" t="inlineStr">
         <is>
           <t>Database</t>
         </is>
       </c>
-      <c r="C12" s="42" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="D12" s="41" t="inlineStr">
+      <c r="C12" s="41" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="D12" s="40" t="inlineStr">
         <is>
           <t>[********]</t>
         </is>
       </c>
-      <c r="E12" s="41" t="inlineStr">
+      <c r="E12" s="40" t="inlineStr">
         <is>
           <t>Database connection password</t>
         </is>
       </c>
-      <c r="F12" s="42" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G12" s="41" t="inlineStr">
+      <c r="F12" s="41" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G12" s="40" t="inlineStr">
         <is>
           <t>String</t>
         </is>
       </c>
-      <c r="H12" s="41" t="inlineStr">
+      <c r="H12" s="40" t="inlineStr">
         <is>
           <t>Min 12 chars with complexity</t>
         </is>
       </c>
-      <c r="I12" s="42" t="inlineStr">
+      <c r="I12" s="41" t="inlineStr">
         <is>
           <t>Secret</t>
         </is>
       </c>
-      <c r="J12" s="41" t="inlineStr">
+      <c r="J12" s="40" t="inlineStr">
         <is>
           <t>Database Team</t>
         </is>
       </c>
-      <c r="K12" s="41" t="inlineStr">
+      <c r="K12" s="40" t="inlineStr">
         <is>
           <t>User creation</t>
         </is>
       </c>
-      <c r="L12" s="41" t="inlineStr">
+      <c r="L12" s="40" t="inlineStr">
         <is>
           <t>Store in secrets manager</t>
         </is>
       </c>
-      <c r="M12" s="42" t="inlineStr">
+      <c r="M12" s="41" t="inlineStr">
         <is>
           <t>[DATE]</t>
         </is>
       </c>
     </row>
     <row r="13" ht="26" customHeight="1">
-      <c r="A13" s="37" t="inlineStr">
+      <c r="A13" s="36" t="inlineStr">
         <is>
           <t>DB_SSL_MODE</t>
         </is>
       </c>
-      <c r="B13" s="38" t="inlineStr">
+      <c r="B13" s="37" t="inlineStr">
         <is>
           <t>Database</t>
         </is>
       </c>
-      <c r="C13" s="39" t="inlineStr">
+      <c r="C13" s="38" t="inlineStr">
         <is>
           <t>Production</t>
         </is>
       </c>
-      <c r="D13" s="38" t="inlineStr">
+      <c r="D13" s="37" t="inlineStr">
         <is>
           <t>[********]</t>
         </is>
       </c>
-      <c r="E13" s="38" t="inlineStr">
+      <c r="E13" s="37" t="inlineStr">
         <is>
           <t>SSL connection requirement</t>
         </is>
       </c>
-      <c r="F13" s="39" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G13" s="38" t="inlineStr">
+      <c r="F13" s="38" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G13" s="37" t="inlineStr">
         <is>
           <t>String</t>
         </is>
       </c>
-      <c r="H13" s="38" t="inlineStr">
+      <c r="H13" s="37" t="inlineStr">
         <is>
           <t>disable|allow|prefer|require</t>
         </is>
       </c>
-      <c r="I13" s="39" t="inlineStr">
+      <c r="I13" s="38" t="inlineStr">
         <is>
           <t>Confidential</t>
         </is>
       </c>
-      <c r="J13" s="38" t="inlineStr">
+      <c r="J13" s="37" t="inlineStr">
         <is>
           <t>Security Team</t>
         </is>
       </c>
-      <c r="K13" s="38" t="inlineStr">
+      <c r="K13" s="37" t="inlineStr">
         <is>
           <t>SSL certificates</t>
         </is>
       </c>
-      <c r="L13" s="38" t="inlineStr">
+      <c r="L13" s="37" t="inlineStr">
         <is>
           <t>Always require for production</t>
         </is>
       </c>
-      <c r="M13" s="39" t="inlineStr">
+      <c r="M13" s="38" t="inlineStr">
         <is>
           <t>[DATE]</t>
         </is>
       </c>
     </row>
     <row r="14" ht="26" customHeight="1">
-      <c r="A14" s="40" t="inlineStr">
+      <c r="A14" s="39" t="inlineStr">
         <is>
           <t>DB_POOL_MIN</t>
         </is>
       </c>
-      <c r="B14" s="41" t="inlineStr">
+      <c r="B14" s="40" t="inlineStr">
         <is>
           <t>Database</t>
         </is>
       </c>
-      <c r="C14" s="42" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="D14" s="41" t="inlineStr">
+      <c r="C14" s="41" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="D14" s="40" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
-      <c r="E14" s="41" t="inlineStr">
+      <c r="E14" s="40" t="inlineStr">
         <is>
           <t>Minimum database connections in pool</t>
         </is>
       </c>
-      <c r="F14" s="42" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G14" s="41" t="inlineStr">
+      <c r="F14" s="41" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G14" s="40" t="inlineStr">
         <is>
           <t>Integer</t>
         </is>
       </c>
-      <c r="H14" s="41" t="inlineStr">
+      <c r="H14" s="40" t="inlineStr">
         <is>
           <t>1-100</t>
         </is>
       </c>
-      <c r="I14" s="42" t="inlineStr">
+      <c r="I14" s="41" t="inlineStr">
         <is>
           <t>Public</t>
         </is>
       </c>
-      <c r="J14" s="41" t="inlineStr">
+      <c r="J14" s="40" t="inlineStr">
         <is>
           <t>Database Team</t>
         </is>
       </c>
-      <c r="K14" s="41" t="inlineStr">
+      <c r="K14" s="40" t="inlineStr">
         <is>
           <t>DB_POOL_MAX</t>
         </is>
       </c>
-      <c r="L14" s="41" t="inlineStr">
+      <c r="L14" s="40" t="inlineStr">
         <is>
           <t>Tune based on load patterns</t>
         </is>
       </c>
-      <c r="M14" s="42" t="inlineStr">
+      <c r="M14" s="41" t="inlineStr">
         <is>
           <t>[DATE]</t>
         </is>
       </c>
     </row>
     <row r="15" ht="26" customHeight="1">
-      <c r="A15" s="37" t="inlineStr">
+      <c r="A15" s="36" t="inlineStr">
         <is>
           <t>DB_POOL_MAX</t>
         </is>
       </c>
-      <c r="B15" s="38" t="inlineStr">
+      <c r="B15" s="37" t="inlineStr">
         <is>
           <t>Database</t>
         </is>
       </c>
-      <c r="C15" s="39" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="D15" s="38" t="inlineStr">
+      <c r="C15" s="38" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="D15" s="37" t="inlineStr">
         <is>
           <t>20</t>
         </is>
       </c>
-      <c r="E15" s="38" t="inlineStr">
+      <c r="E15" s="37" t="inlineStr">
         <is>
           <t>Maximum database connections in pool</t>
         </is>
       </c>
-      <c r="F15" s="39" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G15" s="38" t="inlineStr">
+      <c r="F15" s="38" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G15" s="37" t="inlineStr">
         <is>
           <t>Integer</t>
         </is>
       </c>
-      <c r="H15" s="38" t="inlineStr">
+      <c r="H15" s="37" t="inlineStr">
         <is>
           <t>5-500</t>
         </is>
       </c>
-      <c r="I15" s="39" t="inlineStr">
+      <c r="I15" s="38" t="inlineStr">
         <is>
           <t>Public</t>
         </is>
       </c>
-      <c r="J15" s="38" t="inlineStr">
+      <c r="J15" s="37" t="inlineStr">
         <is>
           <t>Database Team</t>
         </is>
       </c>
-      <c r="K15" s="38" t="inlineStr">
+      <c r="K15" s="37" t="inlineStr">
         <is>
           <t>DB_POOL_MIN</t>
         </is>
       </c>
-      <c r="L15" s="38" t="inlineStr">
+      <c r="L15" s="37" t="inlineStr">
         <is>
           <t>Monitor connection usage</t>
         </is>
       </c>
-      <c r="M15" s="39" t="inlineStr">
+      <c r="M15" s="38" t="inlineStr">
         <is>
           <t>[DATE]</t>
         </is>
       </c>
     </row>
     <row r="16" ht="26" customHeight="1">
-      <c r="A16" s="40" t="inlineStr">
+      <c r="A16" s="39" t="inlineStr">
         <is>
           <t>CACHE_HOST</t>
         </is>
       </c>
-      <c r="B16" s="41" t="inlineStr">
+      <c r="B16" s="40" t="inlineStr">
         <is>
           <t>Cache</t>
         </is>
       </c>
-      <c r="C16" s="42" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="D16" s="41" t="inlineStr">
+      <c r="C16" s="41" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="D16" s="40" t="inlineStr">
         <is>
           <t>[********]</t>
         </is>
       </c>
-      <c r="E16" s="41" t="inlineStr">
+      <c r="E16" s="40" t="inlineStr">
         <is>
           <t>Redis cache server hostname</t>
         </is>
       </c>
-      <c r="F16" s="42" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G16" s="41" t="inlineStr">
+      <c r="F16" s="41" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G16" s="40" t="inlineStr">
         <is>
           <t>String</t>
         </is>
       </c>
-      <c r="H16" s="41" t="inlineStr">
+      <c r="H16" s="40" t="inlineStr">
         <is>
           <t>Valid hostname or IP</t>
         </is>
       </c>
-      <c r="I16" s="42" t="inlineStr">
+      <c r="I16" s="41" t="inlineStr">
         <is>
           <t>Confidential</t>
         </is>
       </c>
-      <c r="J16" s="41" t="inlineStr">
+      <c r="J16" s="40" t="inlineStr">
         <is>
           <t>Infrastructure</t>
         </is>
       </c>
-      <c r="K16" s="41" t="inlineStr">
+      <c r="K16" s="40" t="inlineStr">
         <is>
           <t>Network connectivity</t>
         </is>
       </c>
-      <c r="L16" s="41" t="inlineStr">
+      <c r="L16" s="40" t="inlineStr">
         <is>
           <t>Use Redis cluster for HA</t>
         </is>
       </c>
-      <c r="M16" s="42" t="inlineStr">
+      <c r="M16" s="41" t="inlineStr">
         <is>
           <t>[DATE]</t>
         </is>
       </c>
     </row>
     <row r="17" ht="26" customHeight="1">
-      <c r="A17" s="37" t="inlineStr">
+      <c r="A17" s="36" t="inlineStr">
         <is>
           <t>CACHE_PORT</t>
         </is>
       </c>
-      <c r="B17" s="38" t="inlineStr">
+      <c r="B17" s="37" t="inlineStr">
         <is>
           <t>Cache</t>
         </is>
       </c>
-      <c r="C17" s="39" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="D17" s="38" t="inlineStr">
+      <c r="C17" s="38" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="D17" s="37" t="inlineStr">
         <is>
           <t>6379</t>
         </is>
       </c>
-      <c r="E17" s="38" t="inlineStr">
+      <c r="E17" s="37" t="inlineStr">
         <is>
           <t>Redis cache server port</t>
         </is>
       </c>
-      <c r="F17" s="39" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G17" s="38" t="inlineStr">
+      <c r="F17" s="38" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G17" s="37" t="inlineStr">
         <is>
           <t>Integer</t>
         </is>
       </c>
-      <c r="H17" s="38" t="inlineStr">
+      <c r="H17" s="37" t="inlineStr">
         <is>
           <t>1-65535</t>
         </is>
       </c>
-      <c r="I17" s="39" t="inlineStr">
+      <c r="I17" s="38" t="inlineStr">
         <is>
           <t>Public</t>
         </is>
       </c>
-      <c r="J17" s="38" t="inlineStr">
+      <c r="J17" s="37" t="inlineStr">
         <is>
           <t>Infrastructure</t>
         </is>
       </c>
-      <c r="K17" s="38" t="inlineStr">
+      <c r="K17" s="37" t="inlineStr">
         <is>
           <t>Firewall rules</t>
         </is>
       </c>
-      <c r="L17" s="38" t="inlineStr">
+      <c r="L17" s="37" t="inlineStr">
         <is>
           <t>Redis default port</t>
         </is>
       </c>
-      <c r="M17" s="39" t="inlineStr">
+      <c r="M17" s="38" t="inlineStr">
         <is>
           <t>[DATE]</t>
         </is>
       </c>
     </row>
     <row r="18" ht="26" customHeight="1">
-      <c r="A18" s="40" t="inlineStr">
+      <c r="A18" s="39" t="inlineStr">
         <is>
           <t>CACHE_PASSWORD</t>
         </is>
       </c>
-      <c r="B18" s="41" t="inlineStr">
+      <c r="B18" s="40" t="inlineStr">
         <is>
           <t>Cache</t>
         </is>
       </c>
-      <c r="C18" s="42" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="D18" s="41" t="inlineStr">
+      <c r="C18" s="41" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="D18" s="40" t="inlineStr">
         <is>
           <t>[********]</t>
         </is>
       </c>
-      <c r="E18" s="41" t="inlineStr">
+      <c r="E18" s="40" t="inlineStr">
         <is>
           <t>Redis authentication password</t>
         </is>
       </c>
-      <c r="F18" s="42" t="inlineStr">
+      <c r="F18" s="41" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="G18" s="41" t="inlineStr">
+      <c r="G18" s="40" t="inlineStr">
         <is>
           <t>String</t>
         </is>
       </c>
-      <c r="H18" s="41" t="inlineStr">
+      <c r="H18" s="40" t="inlineStr">
         <is>
           <t>Min 8 characters</t>
         </is>
       </c>
-      <c r="I18" s="42" t="inlineStr">
+      <c r="I18" s="41" t="inlineStr">
         <is>
           <t>Secret</t>
         </is>
       </c>
-      <c r="J18" s="41" t="inlineStr">
+      <c r="J18" s="40" t="inlineStr">
         <is>
           <t>Infrastructure</t>
         </is>
       </c>
-      <c r="K18" s="41" t="inlineStr">
+      <c r="K18" s="40" t="inlineStr">
         <is>
           <t>Redis configuration</t>
         </is>
       </c>
-      <c r="L18" s="41" t="inlineStr">
+      <c r="L18" s="40" t="inlineStr">
         <is>
           <t>Optional if Redis AUTH disabled</t>
         </is>
       </c>
-      <c r="M18" s="42" t="inlineStr">
+      <c r="M18" s="41" t="inlineStr">
         <is>
           <t>[DATE]</t>
         </is>
       </c>
     </row>
     <row r="19" ht="26" customHeight="1">
-      <c r="A19" s="37" t="inlineStr">
+      <c r="A19" s="36" t="inlineStr">
         <is>
           <t>CACHE_TTL</t>
         </is>
       </c>
-      <c r="B19" s="38" t="inlineStr">
+      <c r="B19" s="37" t="inlineStr">
         <is>
           <t>Cache</t>
         </is>
       </c>
-      <c r="C19" s="39" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="D19" s="38" t="inlineStr">
+      <c r="C19" s="38" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="D19" s="37" t="inlineStr">
         <is>
           <t>3600</t>
         </is>
       </c>
-      <c r="E19" s="38" t="inlineStr">
+      <c r="E19" s="37" t="inlineStr">
         <is>
           <t>Default cache time-to-live in seconds</t>
         </is>
       </c>
-      <c r="F19" s="39" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G19" s="38" t="inlineStr">
+      <c r="F19" s="38" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G19" s="37" t="inlineStr">
         <is>
           <t>Integer</t>
         </is>
       </c>
-      <c r="H19" s="38" t="inlineStr">
+      <c r="H19" s="37" t="inlineStr">
         <is>
           <t>60-86400</t>
         </is>
       </c>
-      <c r="I19" s="39" t="inlineStr">
+      <c r="I19" s="38" t="inlineStr">
         <is>
           <t>Public</t>
         </is>
       </c>
-      <c r="J19" s="38" t="inlineStr">
+      <c r="J19" s="37" t="inlineStr">
         <is>
           <t>Development</t>
         </is>
       </c>
-      <c r="K19" s="38" t="inlineStr">
+      <c r="K19" s="37" t="inlineStr">
         <is>
           <t>Cache strategy</t>
         </is>
       </c>
-      <c r="L19" s="38" t="inlineStr">
+      <c r="L19" s="37" t="inlineStr">
         <is>
           <t>Tune based on data patterns</t>
         </is>
       </c>
-      <c r="M19" s="39" t="inlineStr">
+      <c r="M19" s="38" t="inlineStr">
         <is>
           <t>[DATE]</t>
         </is>
       </c>
     </row>
     <row r="20" ht="26" customHeight="1">
-      <c r="A20" s="40" t="inlineStr">
+      <c r="A20" s="39" t="inlineStr">
         <is>
           <t>JWT_SECRET</t>
         </is>
       </c>
-      <c r="B20" s="41" t="inlineStr">
+      <c r="B20" s="40" t="inlineStr">
         <is>
           <t>Security</t>
         </is>
       </c>
-      <c r="C20" s="42" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="D20" s="41" t="inlineStr">
+      <c r="C20" s="41" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="D20" s="40" t="inlineStr">
         <is>
           <t>[********]</t>
         </is>
       </c>
-      <c r="E20" s="41" t="inlineStr">
+      <c r="E20" s="40" t="inlineStr">
         <is>
           <t>Secret key for JWT token signing</t>
         </is>
       </c>
-      <c r="F20" s="42" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G20" s="41" t="inlineStr">
+      <c r="F20" s="41" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G20" s="40" t="inlineStr">
         <is>
           <t>String</t>
         </is>
       </c>
-      <c r="H20" s="41" t="inlineStr">
+      <c r="H20" s="40" t="inlineStr">
         <is>
           <t>Min 32 chars base64</t>
         </is>
       </c>
-      <c r="I20" s="42" t="inlineStr">
+      <c r="I20" s="41" t="inlineStr">
         <is>
           <t>Secret</t>
         </is>
       </c>
-      <c r="J20" s="41" t="inlineStr">
+      <c r="J20" s="40" t="inlineStr">
         <is>
           <t>Security Team</t>
         </is>
       </c>
-      <c r="K20" s="41" t="inlineStr">
+      <c r="K20" s="40" t="inlineStr">
         <is>
           <t>Authentication</t>
         </is>
       </c>
-      <c r="L20" s="41" t="inlineStr">
+      <c r="L20" s="40" t="inlineStr">
         <is>
           <t>Rotate regularly</t>
         </is>
       </c>
-      <c r="M20" s="42" t="inlineStr">
+      <c r="M20" s="41" t="inlineStr">
         <is>
           <t>[DATE]</t>
         </is>
       </c>
     </row>
     <row r="21" ht="26" customHeight="1">
-      <c r="A21" s="37" t="inlineStr">
+      <c r="A21" s="36" t="inlineStr">
         <is>
           <t>ENCRYPTION_KEY</t>
         </is>
       </c>
-      <c r="B21" s="38" t="inlineStr">
+      <c r="B21" s="37" t="inlineStr">
         <is>
           <t>Security</t>
         </is>
       </c>
-      <c r="C21" s="39" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="D21" s="38" t="inlineStr">
+      <c r="C21" s="38" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="D21" s="37" t="inlineStr">
         <is>
           <t>[********]</t>
         </is>
       </c>
-      <c r="E21" s="38" t="inlineStr">
+      <c r="E21" s="37" t="inlineStr">
         <is>
           <t>Key for data encryption at rest</t>
         </is>
       </c>
-      <c r="F21" s="39" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G21" s="38" t="inlineStr">
+      <c r="F21" s="38" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G21" s="37" t="inlineStr">
         <is>
           <t>String</t>
         </is>
       </c>
-      <c r="H21" s="38" t="inlineStr">
+      <c r="H21" s="37" t="inlineStr">
         <is>
           <t>256-bit key base64</t>
         </is>
       </c>
-      <c r="I21" s="39" t="inlineStr">
+      <c r="I21" s="38" t="inlineStr">
         <is>
           <t>Secret</t>
         </is>
       </c>
-      <c r="J21" s="38" t="inlineStr">
+      <c r="J21" s="37" t="inlineStr">
         <is>
           <t>Security Team</t>
         </is>
       </c>
-      <c r="K21" s="38" t="inlineStr">
+      <c r="K21" s="37" t="inlineStr">
         <is>
           <t>Encryption service</t>
         </is>
       </c>
-      <c r="L21" s="38" t="inlineStr">
+      <c r="L21" s="37" t="inlineStr">
         <is>
           <t>Use key management service</t>
         </is>
       </c>
-      <c r="M21" s="39" t="inlineStr">
+      <c r="M21" s="38" t="inlineStr">
         <is>
           <t>[DATE]</t>
         </is>
       </c>
     </row>
     <row r="22" ht="26" customHeight="1">
-      <c r="A22" s="40" t="inlineStr">
+      <c r="A22" s="39" t="inlineStr">
         <is>
           <t>API_KEY</t>
         </is>
       </c>
-      <c r="B22" s="41" t="inlineStr">
+      <c r="B22" s="40" t="inlineStr">
         <is>
           <t>Security</t>
         </is>
       </c>
-      <c r="C22" s="42" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="D22" s="41" t="inlineStr">
+      <c r="C22" s="41" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="D22" s="40" t="inlineStr">
         <is>
           <t>[********]</t>
         </is>
       </c>
-      <c r="E22" s="41" t="inlineStr">
+      <c r="E22" s="40" t="inlineStr">
         <is>
           <t>API authentication key</t>
         </is>
       </c>
-      <c r="F22" s="42" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G22" s="41" t="inlineStr">
+      <c r="F22" s="41" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G22" s="40" t="inlineStr">
         <is>
           <t>String</t>
         </is>
       </c>
-      <c r="H22" s="41" t="inlineStr">
+      <c r="H22" s="40" t="inlineStr">
         <is>
           <t>UUID or secure random</t>
         </is>
       </c>
-      <c r="I22" s="42" t="inlineStr">
+      <c r="I22" s="41" t="inlineStr">
         <is>
           <t>Secret</t>
         </is>
       </c>
-      <c r="J22" s="41" t="inlineStr">
+      <c r="J22" s="40" t="inlineStr">
         <is>
           <t>API Team</t>
         </is>
       </c>
-      <c r="K22" s="41" t="inlineStr">
+      <c r="K22" s="40" t="inlineStr">
         <is>
           <t>External services</t>
         </is>
       </c>
-      <c r="L22" s="41" t="inlineStr">
+      <c r="L22" s="40" t="inlineStr">
         <is>
           <t>Unique per environment</t>
         </is>
       </c>
-      <c r="M22" s="42" t="inlineStr">
+      <c r="M22" s="41" t="inlineStr">
         <is>
           <t>[DATE]</t>
         </is>
       </c>
     </row>
     <row r="23" ht="26" customHeight="1">
-      <c r="A23" s="37" t="inlineStr">
+      <c r="A23" s="36" t="inlineStr">
         <is>
           <t>CORS_ORIGINS</t>
         </is>
       </c>
-      <c r="B23" s="38" t="inlineStr">
+      <c r="B23" s="37" t="inlineStr">
         <is>
           <t>Security</t>
         </is>
       </c>
-      <c r="C23" s="39" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="D23" s="38" t="inlineStr">
+      <c r="C23" s="38" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="D23" s="37" t="inlineStr">
         <is>
           <t>[********]</t>
         </is>
       </c>
-      <c r="E23" s="38" t="inlineStr">
+      <c r="E23" s="37" t="inlineStr">
         <is>
           <t>Allowed CORS origins</t>
         </is>
       </c>
-      <c r="F23" s="39" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G23" s="38" t="inlineStr">
+      <c r="F23" s="38" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G23" s="37" t="inlineStr">
         <is>
           <t>String</t>
         </is>
       </c>
-      <c r="H23" s="38" t="inlineStr">
+      <c r="H23" s="37" t="inlineStr">
         <is>
           <t>Comma-separated URLs</t>
         </is>
       </c>
-      <c r="I23" s="39" t="inlineStr">
+      <c r="I23" s="38" t="inlineStr">
         <is>
           <t>Confidential</t>
         </is>
       </c>
-      <c r="J23" s="38" t="inlineStr">
+      <c r="J23" s="37" t="inlineStr">
         <is>
           <t>Security Team</t>
         </is>
       </c>
-      <c r="K23" s="38" t="inlineStr">
+      <c r="K23" s="37" t="inlineStr">
         <is>
           <t>Frontend domains</t>
         </is>
       </c>
-      <c r="L23" s="38" t="inlineStr">
+      <c r="L23" s="37" t="inlineStr">
         <is>
           <t>Restrict to known domains</t>
         </is>
       </c>
-      <c r="M23" s="39" t="inlineStr">
+      <c r="M23" s="38" t="inlineStr">
         <is>
           <t>[DATE]</t>
         </is>
       </c>
     </row>
     <row r="24" ht="26" customHeight="1">
-      <c r="A24" s="40" t="inlineStr">
+      <c r="A24" s="39" t="inlineStr">
         <is>
           <t>SERVICE_ENDPOINT</t>
         </is>
       </c>
-      <c r="B24" s="41" t="inlineStr">
+      <c r="B24" s="40" t="inlineStr">
         <is>
           <t>Integration</t>
         </is>
       </c>
-      <c r="C24" s="42" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="D24" s="41" t="inlineStr">
+      <c r="C24" s="41" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="D24" s="40" t="inlineStr">
         <is>
           <t>[********]</t>
         </is>
       </c>
-      <c r="E24" s="41" t="inlineStr">
+      <c r="E24" s="40" t="inlineStr">
         <is>
           <t>External service API endpoint</t>
         </is>
       </c>
-      <c r="F24" s="42" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G24" s="41" t="inlineStr">
+      <c r="F24" s="41" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G24" s="40" t="inlineStr">
         <is>
           <t>String</t>
         </is>
       </c>
-      <c r="H24" s="41" t="inlineStr">
+      <c r="H24" s="40" t="inlineStr">
         <is>
           <t>Valid HTTPS URL</t>
         </is>
       </c>
-      <c r="I24" s="42" t="inlineStr">
+      <c r="I24" s="41" t="inlineStr">
         <is>
           <t>Confidential</t>
         </is>
       </c>
-      <c r="J24" s="41" t="inlineStr">
+      <c r="J24" s="40" t="inlineStr">
         <is>
           <t>Integration Team</t>
         </is>
       </c>
-      <c r="K24" s="41" t="inlineStr">
+      <c r="K24" s="40" t="inlineStr">
         <is>
           <t>Service availability</t>
         </is>
       </c>
-      <c r="L24" s="41" t="inlineStr">
+      <c r="L24" s="40" t="inlineStr">
         <is>
           <t>Use load balancer URL</t>
         </is>
       </c>
-      <c r="M24" s="42" t="inlineStr">
+      <c r="M24" s="41" t="inlineStr">
         <is>
           <t>[DATE]</t>
         </is>
       </c>
     </row>
     <row r="25" ht="26" customHeight="1">
-      <c r="A25" s="37" t="inlineStr">
+      <c r="A25" s="36" t="inlineStr">
         <is>
           <t>SERVICE_API_KEY</t>
         </is>
       </c>
-      <c r="B25" s="38" t="inlineStr">
+      <c r="B25" s="37" t="inlineStr">
         <is>
           <t>Integration</t>
         </is>
       </c>
-      <c r="C25" s="39" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="D25" s="38" t="inlineStr">
+      <c r="C25" s="38" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="D25" s="37" t="inlineStr">
         <is>
           <t>[********]</t>
         </is>
       </c>
-      <c r="E25" s="38" t="inlineStr">
+      <c r="E25" s="37" t="inlineStr">
         <is>
           <t>API key for external service</t>
         </is>
       </c>
-      <c r="F25" s="39" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G25" s="38" t="inlineStr">
+      <c r="F25" s="38" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G25" s="37" t="inlineStr">
         <is>
           <t>String</t>
         </is>
       </c>
-      <c r="H25" s="38" t="inlineStr">
+      <c r="H25" s="37" t="inlineStr">
         <is>
           <t>Provider-specific format</t>
         </is>
       </c>
-      <c r="I25" s="39" t="inlineStr">
+      <c r="I25" s="38" t="inlineStr">
         <is>
           <t>Secret</t>
         </is>
       </c>
-      <c r="J25" s="38" t="inlineStr">
+      <c r="J25" s="37" t="inlineStr">
         <is>
           <t>Integration Team</t>
         </is>
       </c>
-      <c r="K25" s="38" t="inlineStr">
+      <c r="K25" s="37" t="inlineStr">
         <is>
           <t>Service registration</t>
         </is>
       </c>
-      <c r="L25" s="38" t="inlineStr">
+      <c r="L25" s="37" t="inlineStr">
         <is>
           <t>Obtain from service provider</t>
         </is>
       </c>
-      <c r="M25" s="39" t="inlineStr">
+      <c r="M25" s="38" t="inlineStr">
         <is>
           <t>[DATE]</t>
         </is>
       </c>
     </row>
     <row r="26" ht="26" customHeight="1">
-      <c r="A26" s="40" t="inlineStr">
+      <c r="A26" s="39" t="inlineStr">
         <is>
           <t>SERVICE_TIMEOUT</t>
         </is>
       </c>
-      <c r="B26" s="41" t="inlineStr">
+      <c r="B26" s="40" t="inlineStr">
         <is>
           <t>Integration</t>
         </is>
       </c>
-      <c r="C26" s="42" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="D26" s="41" t="inlineStr">
+      <c r="C26" s="41" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="D26" s="40" t="inlineStr">
         <is>
           <t>30000</t>
         </is>
       </c>
-      <c r="E26" s="41" t="inlineStr">
+      <c r="E26" s="40" t="inlineStr">
         <is>
           <t>Service call timeout in milliseconds</t>
         </is>
       </c>
-      <c r="F26" s="42" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G26" s="41" t="inlineStr">
+      <c r="F26" s="41" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G26" s="40" t="inlineStr">
         <is>
           <t>Integer</t>
         </is>
       </c>
-      <c r="H26" s="41" t="inlineStr">
+      <c r="H26" s="40" t="inlineStr">
         <is>
           <t>1000-300000</t>
         </is>
       </c>
-      <c r="I26" s="42" t="inlineStr">
+      <c r="I26" s="41" t="inlineStr">
         <is>
           <t>Public</t>
         </is>
       </c>
-      <c r="J26" s="41" t="inlineStr">
+      <c r="J26" s="40" t="inlineStr">
         <is>
           <t>Integration Team</t>
         </is>
       </c>
-      <c r="K26" s="41" t="inlineStr">
+      <c r="K26" s="40" t="inlineStr">
         <is>
           <t>Network latency</t>
         </is>
       </c>
-      <c r="L26" s="41" t="inlineStr">
+      <c r="L26" s="40" t="inlineStr">
         <is>
           <t>Adjust based on SLA</t>
         </is>
       </c>
-      <c r="M26" s="42" t="inlineStr">
+      <c r="M26" s="41" t="inlineStr">
         <is>
           <t>[DATE]</t>
         </is>
       </c>
     </row>
     <row r="27" ht="26" customHeight="1">
-      <c r="A27" s="37" t="inlineStr">
+      <c r="A27" s="36" t="inlineStr">
         <is>
           <t>METRICS_ENABLED</t>
         </is>
       </c>
-      <c r="B27" s="38" t="inlineStr">
+      <c r="B27" s="37" t="inlineStr">
         <is>
           <t>Monitoring</t>
         </is>
       </c>
-      <c r="C27" s="39" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="D27" s="38" t="inlineStr">
+      <c r="C27" s="38" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="D27" s="37" t="inlineStr">
         <is>
           <t>true</t>
         </is>
       </c>
-      <c r="E27" s="38" t="inlineStr">
+      <c r="E27" s="37" t="inlineStr">
         <is>
           <t>Enable metrics collection</t>
         </is>
       </c>
-      <c r="F27" s="39" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G27" s="38" t="inlineStr">
+      <c r="F27" s="38" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G27" s="37" t="inlineStr">
         <is>
           <t>Boolean</t>
         </is>
       </c>
-      <c r="H27" s="38" t="inlineStr">
+      <c r="H27" s="37" t="inlineStr">
         <is>
           <t>true|false</t>
         </is>
       </c>
-      <c r="I27" s="39" t="inlineStr">
+      <c r="I27" s="38" t="inlineStr">
         <is>
           <t>Public</t>
         </is>
       </c>
-      <c r="J27" s="38" t="inlineStr">
+      <c r="J27" s="37" t="inlineStr">
         <is>
           <t>Operations</t>
         </is>
       </c>
-      <c r="K27" s="38" t="inlineStr">
+      <c r="K27" s="37" t="inlineStr">
         <is>
           <t>Monitoring tools</t>
         </is>
       </c>
-      <c r="L27" s="38" t="inlineStr">
+      <c r="L27" s="37" t="inlineStr">
         <is>
           <t>Always enable for production</t>
         </is>
       </c>
-      <c r="M27" s="39" t="inlineStr">
+      <c r="M27" s="38" t="inlineStr">
         <is>
           <t>[DATE]</t>
         </is>
       </c>
     </row>
     <row r="28" ht="26" customHeight="1">
-      <c r="A28" s="40" t="inlineStr">
+      <c r="A28" s="39" t="inlineStr">
         <is>
           <t>HEALTH_CHECK_PATH</t>
         </is>
       </c>
-      <c r="B28" s="41" t="inlineStr">
+      <c r="B28" s="40" t="inlineStr">
         <is>
           <t>Monitoring</t>
         </is>
       </c>
-      <c r="C28" s="42" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="D28" s="41" t="inlineStr">
+      <c r="C28" s="41" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="D28" s="40" t="inlineStr">
         <is>
           <t>/health</t>
         </is>
       </c>
-      <c r="E28" s="41" t="inlineStr">
+      <c r="E28" s="40" t="inlineStr">
         <is>
           <t>Health check endpoint path</t>
         </is>
       </c>
-      <c r="F28" s="42" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G28" s="41" t="inlineStr">
+      <c r="F28" s="41" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G28" s="40" t="inlineStr">
         <is>
           <t>String</t>
         </is>
       </c>
-      <c r="H28" s="41" t="inlineStr">
+      <c r="H28" s="40" t="inlineStr">
         <is>
           <t>Valid URL path</t>
         </is>
       </c>
-      <c r="I28" s="42" t="inlineStr">
+      <c r="I28" s="41" t="inlineStr">
         <is>
           <t>Public</t>
         </is>
       </c>
-      <c r="J28" s="41" t="inlineStr">
+      <c r="J28" s="40" t="inlineStr">
         <is>
           <t>Operations</t>
         </is>
       </c>
-      <c r="K28" s="41" t="inlineStr">
+      <c r="K28" s="40" t="inlineStr">
         <is>
           <t>Load balancer</t>
         </is>
       </c>
-      <c r="L28" s="41" t="inlineStr">
+      <c r="L28" s="40" t="inlineStr">
         <is>
           <t>Must return 200 for healthy</t>
         </is>
       </c>
-      <c r="M28" s="42" t="inlineStr">
+      <c r="M28" s="41" t="inlineStr">
         <is>
           <t>[DATE]</t>
         </is>
       </c>
     </row>
     <row r="29" ht="26" customHeight="1">
-      <c r="A29" s="37" t="inlineStr">
+      <c r="A29" s="36" t="inlineStr">
         <is>
           <t>PROMETHEUS_PORT</t>
         </is>
       </c>
-      <c r="B29" s="38" t="inlineStr">
+      <c r="B29" s="37" t="inlineStr">
         <is>
           <t>Monitoring</t>
         </is>
       </c>
-      <c r="C29" s="39" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="D29" s="38" t="inlineStr">
+      <c r="C29" s="38" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="D29" s="37" t="inlineStr">
         <is>
           <t>9090</t>
         </is>
       </c>
-      <c r="E29" s="38" t="inlineStr">
+      <c r="E29" s="37" t="inlineStr">
         <is>
           <t>Port for Prometheus metrics</t>
         </is>
       </c>
-      <c r="F29" s="39" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G29" s="38" t="inlineStr">
+      <c r="F29" s="38" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G29" s="37" t="inlineStr">
         <is>
           <t>Integer</t>
         </is>
       </c>
-      <c r="H29" s="38" t="inlineStr">
+      <c r="H29" s="37" t="inlineStr">
         <is>
           <t>1024-65535</t>
         </is>
       </c>
-      <c r="I29" s="39" t="inlineStr">
+      <c r="I29" s="38" t="inlineStr">
         <is>
           <t>Public</t>
         </is>
       </c>
-      <c r="J29" s="38" t="inlineStr">
+      <c r="J29" s="37" t="inlineStr">
         <is>
           <t>Operations</t>
         </is>
       </c>
-      <c r="K29" s="38" t="inlineStr">
+      <c r="K29" s="37" t="inlineStr">
         <is>
           <t>Monitoring stack</t>
         </is>
       </c>
-      <c r="L29" s="38" t="inlineStr">
+      <c r="L29" s="37" t="inlineStr">
         <is>
           <t>Ensure port availability</t>
         </is>
       </c>
-      <c r="M29" s="39" t="inlineStr">
+      <c r="M29" s="38" t="inlineStr">
         <is>
           <t>[DATE]</t>
         </is>
       </c>
     </row>
     <row r="30" ht="26" customHeight="1">
-      <c r="A30" s="40" t="inlineStr">
+      <c r="A30" s="39" t="inlineStr">
         <is>
           <t>VPC_CIDR</t>
         </is>
       </c>
-      <c r="B30" s="41" t="inlineStr">
+      <c r="B30" s="40" t="inlineStr">
         <is>
           <t>Network</t>
         </is>
       </c>
-      <c r="C30" s="42" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="D30" s="41" t="inlineStr">
+      <c r="C30" s="41" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="D30" s="40" t="inlineStr">
         <is>
           <t>10.0.0.0/16</t>
         </is>
       </c>
-      <c r="E30" s="41" t="inlineStr">
+      <c r="E30" s="40" t="inlineStr">
         <is>
           <t>VPC CIDR block</t>
         </is>
       </c>
-      <c r="F30" s="42" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G30" s="41" t="inlineStr">
+      <c r="F30" s="41" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G30" s="40" t="inlineStr">
         <is>
           <t>String</t>
         </is>
       </c>
-      <c r="H30" s="41" t="inlineStr">
+      <c r="H30" s="40" t="inlineStr">
         <is>
           <t>Valid CIDR notation</t>
         </is>
       </c>
-      <c r="I30" s="42" t="inlineStr">
+      <c r="I30" s="41" t="inlineStr">
         <is>
           <t>Public</t>
         </is>
       </c>
-      <c r="J30" s="41" t="inlineStr">
+      <c r="J30" s="40" t="inlineStr">
         <is>
           <t>Network Team</t>
         </is>
       </c>
-      <c r="K30" s="41" t="inlineStr">
+      <c r="K30" s="40" t="inlineStr">
         <is>
           <t>IP planning</t>
         </is>
       </c>
-      <c r="L30" s="41" t="inlineStr">
+      <c r="L30" s="40" t="inlineStr">
         <is>
           <t>Plan for future growth</t>
         </is>
       </c>
-      <c r="M30" s="42" t="inlineStr">
+      <c r="M30" s="41" t="inlineStr">
         <is>
           <t>[DATE]</t>
         </is>
       </c>
     </row>
     <row r="31" ht="26" customHeight="1">
-      <c r="A31" s="37" t="inlineStr">
+      <c r="A31" s="36" t="inlineStr">
         <is>
           <t>PUBLIC_SUBNET_1</t>
         </is>
       </c>
-      <c r="B31" s="38" t="inlineStr">
+      <c r="B31" s="37" t="inlineStr">
         <is>
           <t>Network</t>
         </is>
       </c>
-      <c r="C31" s="39" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="D31" s="38" t="inlineStr">
+      <c r="C31" s="38" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="D31" s="37" t="inlineStr">
         <is>
           <t>10.0.1.0/24</t>
         </is>
       </c>
-      <c r="E31" s="38" t="inlineStr">
+      <c r="E31" s="37" t="inlineStr">
         <is>
           <t>First public subnet CIDR</t>
         </is>
       </c>
-      <c r="F31" s="39" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G31" s="38" t="inlineStr">
+      <c r="F31" s="38" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G31" s="37" t="inlineStr">
         <is>
           <t>String</t>
         </is>
       </c>
-      <c r="H31" s="38" t="inlineStr">
+      <c r="H31" s="37" t="inlineStr">
         <is>
           <t>Valid CIDR notation</t>
         </is>
       </c>
-      <c r="I31" s="39" t="inlineStr">
+      <c r="I31" s="38" t="inlineStr">
         <is>
           <t>Public</t>
         </is>
       </c>
-      <c r="J31" s="38" t="inlineStr">
+      <c r="J31" s="37" t="inlineStr">
         <is>
           <t>Network Team</t>
         </is>
       </c>
-      <c r="K31" s="38" t="inlineStr">
+      <c r="K31" s="37" t="inlineStr">
         <is>
           <t>VPC_CIDR</t>
         </is>
       </c>
-      <c r="L31" s="38" t="inlineStr">
+      <c r="L31" s="37" t="inlineStr">
         <is>
           <t>Must be within VPC CIDR</t>
         </is>
       </c>
-      <c r="M31" s="39" t="inlineStr">
+      <c r="M31" s="38" t="inlineStr">
         <is>
           <t>[DATE]</t>
         </is>
       </c>
     </row>
     <row r="32" ht="26" customHeight="1">
-      <c r="A32" s="40" t="inlineStr">
+      <c r="A32" s="39" t="inlineStr">
         <is>
           <t>PUBLIC_SUBNET_2</t>
         </is>
       </c>
-      <c r="B32" s="41" t="inlineStr">
+      <c r="B32" s="40" t="inlineStr">
         <is>
           <t>Network</t>
         </is>
       </c>
-      <c r="C32" s="42" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="D32" s="41" t="inlineStr">
+      <c r="C32" s="41" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="D32" s="40" t="inlineStr">
         <is>
           <t>10.0.2.0/24</t>
         </is>
       </c>
-      <c r="E32" s="41" t="inlineStr">
+      <c r="E32" s="40" t="inlineStr">
         <is>
           <t>Second public subnet CIDR</t>
         </is>
       </c>
-      <c r="F32" s="42" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G32" s="41" t="inlineStr">
+      <c r="F32" s="41" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G32" s="40" t="inlineStr">
         <is>
           <t>String</t>
         </is>
       </c>
-      <c r="H32" s="41" t="inlineStr">
+      <c r="H32" s="40" t="inlineStr">
         <is>
           <t>Valid CIDR notation</t>
         </is>
       </c>
-      <c r="I32" s="42" t="inlineStr">
+      <c r="I32" s="41" t="inlineStr">
         <is>
           <t>Public</t>
         </is>
       </c>
-      <c r="J32" s="41" t="inlineStr">
+      <c r="J32" s="40" t="inlineStr">
         <is>
           <t>Network Team</t>
         </is>
       </c>
-      <c r="K32" s="41" t="inlineStr">
+      <c r="K32" s="40" t="inlineStr">
         <is>
           <t>VPC_CIDR</t>
         </is>
       </c>
-      <c r="L32" s="41" t="inlineStr">
+      <c r="L32" s="40" t="inlineStr">
         <is>
           <t>Different AZ from subnet 1</t>
         </is>
       </c>
-      <c r="M32" s="42" t="inlineStr">
+      <c r="M32" s="41" t="inlineStr">
         <is>
           <t>[DATE]</t>
         </is>
       </c>
     </row>
     <row r="33" ht="26" customHeight="1">
-      <c r="A33" s="37" t="inlineStr">
+      <c r="A33" s="36" t="inlineStr">
         <is>
           <t>PRIVATE_SUBNET_1</t>
         </is>
       </c>
-      <c r="B33" s="38" t="inlineStr">
+      <c r="B33" s="37" t="inlineStr">
         <is>
           <t>Network</t>
         </is>
       </c>
-      <c r="C33" s="39" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="D33" s="38" t="inlineStr">
+      <c r="C33" s="38" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="D33" s="37" t="inlineStr">
         <is>
           <t>10.0.10.0/24</t>
         </is>
       </c>
-      <c r="E33" s="38" t="inlineStr">
+      <c r="E33" s="37" t="inlineStr">
         <is>
           <t>First private subnet CIDR</t>
         </is>
       </c>
-      <c r="F33" s="39" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G33" s="38" t="inlineStr">
+      <c r="F33" s="38" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G33" s="37" t="inlineStr">
         <is>
           <t>String</t>
         </is>
       </c>
-      <c r="H33" s="38" t="inlineStr">
+      <c r="H33" s="37" t="inlineStr">
         <is>
           <t>Valid CIDR notation</t>
         </is>
       </c>
-      <c r="I33" s="39" t="inlineStr">
+      <c r="I33" s="38" t="inlineStr">
         <is>
           <t>Public</t>
         </is>
       </c>
-      <c r="J33" s="38" t="inlineStr">
+      <c r="J33" s="37" t="inlineStr">
         <is>
           <t>Network Team</t>
         </is>
       </c>
-      <c r="K33" s="38" t="inlineStr">
+      <c r="K33" s="37" t="inlineStr">
         <is>
           <t>VPC_CIDR</t>
         </is>
       </c>
-      <c r="L33" s="38" t="inlineStr">
+      <c r="L33" s="37" t="inlineStr">
         <is>
           <t>Must be within VPC CIDR</t>
         </is>
       </c>
-      <c r="M33" s="39" t="inlineStr">
+      <c r="M33" s="38" t="inlineStr">
         <is>
           <t>[DATE]</t>
         </is>
       </c>
     </row>
     <row r="34" ht="26" customHeight="1">
-      <c r="A34" s="40" t="inlineStr">
+      <c r="A34" s="39" t="inlineStr">
         <is>
           <t>PRIVATE_SUBNET_2</t>
         </is>
       </c>
-      <c r="B34" s="41" t="inlineStr">
+      <c r="B34" s="40" t="inlineStr">
         <is>
           <t>Network</t>
         </is>
       </c>
-      <c r="C34" s="42" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="D34" s="41" t="inlineStr">
+      <c r="C34" s="41" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="D34" s="40" t="inlineStr">
         <is>
           <t>10.0.11.0/24</t>
         </is>
       </c>
-      <c r="E34" s="41" t="inlineStr">
+      <c r="E34" s="40" t="inlineStr">
         <is>
           <t>Second private subnet CIDR</t>
         </is>
       </c>
-      <c r="F34" s="42" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G34" s="41" t="inlineStr">
+      <c r="F34" s="41" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G34" s="40" t="inlineStr">
         <is>
           <t>String</t>
         </is>
       </c>
-      <c r="H34" s="41" t="inlineStr">
+      <c r="H34" s="40" t="inlineStr">
         <is>
           <t>Valid CIDR notation</t>
         </is>
       </c>
-      <c r="I34" s="42" t="inlineStr">
+      <c r="I34" s="41" t="inlineStr">
         <is>
           <t>Public</t>
         </is>
       </c>
-      <c r="J34" s="41" t="inlineStr">
+      <c r="J34" s="40" t="inlineStr">
         <is>
           <t>Network Team</t>
         </is>
       </c>
-      <c r="K34" s="41" t="inlineStr">
+      <c r="K34" s="40" t="inlineStr">
         <is>
           <t>VPC_CIDR</t>
         </is>
       </c>
-      <c r="L34" s="41" t="inlineStr">
+      <c r="L34" s="40" t="inlineStr">
         <is>
           <t>Different AZ from subnet 1</t>
         </is>
       </c>
-      <c r="M34" s="42" t="inlineStr">
+      <c r="M34" s="41" t="inlineStr">
         <is>
           <t>[DATE]</t>
         </is>
       </c>
     </row>
     <row r="35" ht="26" customHeight="1">
-      <c r="A35" s="37" t="inlineStr">
+      <c r="A35" s="36" t="inlineStr">
         <is>
           <t>DB_SUBNET_1</t>
         </is>
       </c>
-      <c r="B35" s="38" t="inlineStr">
+      <c r="B35" s="37" t="inlineStr">
         <is>
           <t>Network</t>
         </is>
       </c>
-      <c r="C35" s="39" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="D35" s="38" t="inlineStr">
+      <c r="C35" s="38" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="D35" s="37" t="inlineStr">
         <is>
           <t>10.0.20.0/24</t>
         </is>
       </c>
-      <c r="E35" s="38" t="inlineStr">
+      <c r="E35" s="37" t="inlineStr">
         <is>
           <t>First database subnet CIDR</t>
         </is>
       </c>
-      <c r="F35" s="39" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G35" s="38" t="inlineStr">
+      <c r="F35" s="38" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G35" s="37" t="inlineStr">
         <is>
           <t>String</t>
         </is>
       </c>
-      <c r="H35" s="38" t="inlineStr">
+      <c r="H35" s="37" t="inlineStr">
         <is>
           <t>Valid CIDR notation</t>
         </is>
       </c>
-      <c r="I35" s="39" t="inlineStr">
+      <c r="I35" s="38" t="inlineStr">
         <is>
           <t>Public</t>
         </is>
       </c>
-      <c r="J35" s="38" t="inlineStr">
+      <c r="J35" s="37" t="inlineStr">
         <is>
           <t>Network Team</t>
         </is>
       </c>
-      <c r="K35" s="38" t="inlineStr">
+      <c r="K35" s="37" t="inlineStr">
         <is>
           <t>VPC_CIDR</t>
         </is>
       </c>
-      <c r="L35" s="38" t="inlineStr">
+      <c r="L35" s="37" t="inlineStr">
         <is>
           <t>Isolated database tier</t>
         </is>
       </c>
-      <c r="M35" s="39" t="inlineStr">
+      <c r="M35" s="38" t="inlineStr">
         <is>
           <t>[DATE]</t>
         </is>
       </c>
     </row>
     <row r="36" ht="26" customHeight="1">
-      <c r="A36" s="40" t="inlineStr">
+      <c r="A36" s="39" t="inlineStr">
         <is>
           <t>DB_SUBNET_2</t>
         </is>
       </c>
-      <c r="B36" s="41" t="inlineStr">
+      <c r="B36" s="40" t="inlineStr">
         <is>
           <t>Network</t>
         </is>
       </c>
-      <c r="C36" s="42" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="D36" s="41" t="inlineStr">
+      <c r="C36" s="41" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="D36" s="40" t="inlineStr">
         <is>
           <t>10.0.21.0/24</t>
         </is>
       </c>
-      <c r="E36" s="41" t="inlineStr">
+      <c r="E36" s="40" t="inlineStr">
         <is>
           <t>Second database subnet CIDR</t>
         </is>
       </c>
-      <c r="F36" s="42" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G36" s="41" t="inlineStr">
+      <c r="F36" s="41" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G36" s="40" t="inlineStr">
         <is>
           <t>String</t>
         </is>
       </c>
-      <c r="H36" s="41" t="inlineStr">
+      <c r="H36" s="40" t="inlineStr">
         <is>
           <t>Valid CIDR notation</t>
         </is>
       </c>
-      <c r="I36" s="42" t="inlineStr">
+      <c r="I36" s="41" t="inlineStr">
         <is>
           <t>Public</t>
         </is>
       </c>
-      <c r="J36" s="41" t="inlineStr">
+      <c r="J36" s="40" t="inlineStr">
         <is>
           <t>Network Team</t>
         </is>
       </c>
-      <c r="K36" s="41" t="inlineStr">
+      <c r="K36" s="40" t="inlineStr">
         <is>
           <t>VPC_CIDR</t>
         </is>
       </c>
-      <c r="L36" s="41" t="inlineStr">
+      <c r="L36" s="40" t="inlineStr">
         <is>
           <t>Different AZ from subnet 1</t>
         </is>
       </c>
-      <c r="M36" s="42" t="inlineStr">
+      <c r="M36" s="41" t="inlineStr">
         <is>
           <t>[DATE]</t>
         </is>
       </c>
     </row>
     <row r="37" ht="26" customHeight="1">
-      <c r="A37" s="37" t="inlineStr">
+      <c r="A37" s="36" t="inlineStr">
         <is>
           <t>BACKUP_RETENTION</t>
         </is>
       </c>
-      <c r="B37" s="38" t="inlineStr">
+      <c r="B37" s="37" t="inlineStr">
         <is>
           <t>Operations</t>
         </is>
       </c>
-      <c r="C37" s="39" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="D37" s="38" t="inlineStr">
+      <c r="C37" s="38" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="D37" s="37" t="inlineStr">
         <is>
           <t>30</t>
         </is>
       </c>
-      <c r="E37" s="38" t="inlineStr">
+      <c r="E37" s="37" t="inlineStr">
         <is>
           <t>Backup retention period in days</t>
         </is>
       </c>
-      <c r="F37" s="39" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G37" s="38" t="inlineStr">
+      <c r="F37" s="38" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G37" s="37" t="inlineStr">
         <is>
           <t>Integer</t>
         </is>
       </c>
-      <c r="H37" s="38" t="inlineStr">
+      <c r="H37" s="37" t="inlineStr">
         <is>
           <t>7-365</t>
         </is>
       </c>
-      <c r="I37" s="39" t="inlineStr">
+      <c r="I37" s="38" t="inlineStr">
         <is>
           <t>Public</t>
         </is>
       </c>
-      <c r="J37" s="38" t="inlineStr">
+      <c r="J37" s="37" t="inlineStr">
         <is>
           <t>Operations</t>
         </is>
       </c>
-      <c r="K37" s="38" t="inlineStr">
+      <c r="K37" s="37" t="inlineStr">
         <is>
           <t>Backup strategy</t>
         </is>
       </c>
-      <c r="L37" s="38" t="inlineStr">
+      <c r="L37" s="37" t="inlineStr">
         <is>
           <t>Comply with data policies</t>
         </is>
       </c>
-      <c r="M37" s="39" t="inlineStr">
+      <c r="M37" s="38" t="inlineStr">
         <is>
           <t>[DATE]</t>
         </is>
       </c>
     </row>
     <row r="38" ht="26" customHeight="1">
-      <c r="A38" s="40" t="inlineStr">
+      <c r="A38" s="39" t="inlineStr">
         <is>
           <t>BACKUP_SCHEDULE</t>
         </is>
       </c>
-      <c r="B38" s="41" t="inlineStr">
+      <c r="B38" s="40" t="inlineStr">
         <is>
           <t>Operations</t>
         </is>
       </c>
-      <c r="C38" s="42" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="D38" s="41" t="inlineStr">
+      <c r="C38" s="41" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="D38" s="40" t="inlineStr">
         <is>
           <t>0 2 * * *</t>
         </is>
       </c>
-      <c r="E38" s="41" t="inlineStr">
+      <c r="E38" s="40" t="inlineStr">
         <is>
           <t>Backup schedule in cron format</t>
         </is>
       </c>
-      <c r="F38" s="42" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G38" s="41" t="inlineStr">
+      <c r="F38" s="41" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G38" s="40" t="inlineStr">
         <is>
           <t>String</t>
         </is>
       </c>
-      <c r="H38" s="41" t="inlineStr">
+      <c r="H38" s="40" t="inlineStr">
         <is>
           <t>Valid cron expression</t>
         </is>
       </c>
-      <c r="I38" s="42" t="inlineStr">
+      <c r="I38" s="41" t="inlineStr">
         <is>
           <t>Public</t>
         </is>
       </c>
-      <c r="J38" s="41" t="inlineStr">
+      <c r="J38" s="40" t="inlineStr">
         <is>
           <t>Operations</t>
         </is>
       </c>
-      <c r="K38" s="41" t="inlineStr">
+      <c r="K38" s="40" t="inlineStr">
         <is>
           <t>Backup service</t>
         </is>
       </c>
-      <c r="L38" s="41" t="inlineStr">
+      <c r="L38" s="40" t="inlineStr">
         <is>
           <t>Daily at 2 AM UTC</t>
         </is>
       </c>
-      <c r="M38" s="42" t="inlineStr">
+      <c r="M38" s="41" t="inlineStr">
         <is>
           <t>[DATE]</t>
         </is>
       </c>
     </row>
     <row r="39" ht="26" customHeight="1">
-      <c r="A39" s="37" t="inlineStr">
+      <c r="A39" s="36" t="inlineStr">
         <is>
           <t>LOG_RETENTION</t>
         </is>
       </c>
-      <c r="B39" s="38" t="inlineStr">
+      <c r="B39" s="37" t="inlineStr">
         <is>
           <t>Operations</t>
         </is>
       </c>
-      <c r="C39" s="39" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="D39" s="38" t="inlineStr">
+      <c r="C39" s="38" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="D39" s="37" t="inlineStr">
         <is>
           <t>90</t>
         </is>
       </c>
-      <c r="E39" s="38" t="inlineStr">
+      <c r="E39" s="37" t="inlineStr">
         <is>
           <t>Log retention period in days</t>
         </is>
       </c>
-      <c r="F39" s="39" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G39" s="38" t="inlineStr">
+      <c r="F39" s="38" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G39" s="37" t="inlineStr">
         <is>
           <t>Integer</t>
         </is>
       </c>
-      <c r="H39" s="38" t="inlineStr">
+      <c r="H39" s="37" t="inlineStr">
         <is>
           <t>30-365</t>
         </is>
       </c>
-      <c r="I39" s="39" t="inlineStr">
+      <c r="I39" s="38" t="inlineStr">
         <is>
           <t>Public</t>
         </is>
       </c>
-      <c r="J39" s="38" t="inlineStr">
+      <c r="J39" s="37" t="inlineStr">
         <is>
           <t>Operations</t>
         </is>
       </c>
-      <c r="K39" s="38" t="inlineStr">
+      <c r="K39" s="37" t="inlineStr">
         <is>
           <t>Log management</t>
         </is>
       </c>
-      <c r="L39" s="38" t="inlineStr">
+      <c r="L39" s="37" t="inlineStr">
         <is>
           <t>Balance cost and compliance</t>
         </is>
       </c>
-      <c r="M39" s="39" t="inlineStr">
+      <c r="M39" s="38" t="inlineStr">
         <is>
           <t>[DATE]</t>
         </is>
       </c>
     </row>
     <row r="40" ht="26" customHeight="1">
-      <c r="A40" s="40" t="inlineStr">
+      <c r="A40" s="39" t="inlineStr">
         <is>
           <t>SCALING_MIN_INSTANCES</t>
         </is>
       </c>
-      <c r="B40" s="41" t="inlineStr">
+      <c r="B40" s="40" t="inlineStr">
         <is>
           <t>Operations</t>
         </is>
       </c>
-      <c r="C40" s="42" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="D40" s="41" t="inlineStr">
+      <c r="C40" s="41" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="D40" s="40" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="E40" s="41" t="inlineStr">
+      <c r="E40" s="40" t="inlineStr">
         <is>
           <t>Minimum number of instances</t>
         </is>
       </c>
-      <c r="F40" s="42" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G40" s="41" t="inlineStr">
+      <c r="F40" s="41" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G40" s="40" t="inlineStr">
         <is>
           <t>Integer</t>
         </is>
       </c>
-      <c r="H40" s="41" t="inlineStr">
+      <c r="H40" s="40" t="inlineStr">
         <is>
           <t>1-10</t>
         </is>
       </c>
-      <c r="I40" s="42" t="inlineStr">
+      <c r="I40" s="41" t="inlineStr">
         <is>
           <t>Public</t>
         </is>
       </c>
-      <c r="J40" s="41" t="inlineStr">
+      <c r="J40" s="40" t="inlineStr">
         <is>
           <t>Operations</t>
         </is>
       </c>
-      <c r="K40" s="41" t="inlineStr">
+      <c r="K40" s="40" t="inlineStr">
         <is>
           <t>Load balancer</t>
         </is>
       </c>
-      <c r="L40" s="41" t="inlineStr">
+      <c r="L40" s="40" t="inlineStr">
         <is>
           <t>Ensure high availability</t>
         </is>
       </c>
-      <c r="M40" s="42" t="inlineStr">
+      <c r="M40" s="41" t="inlineStr">
         <is>
           <t>[DATE]</t>
         </is>
       </c>
     </row>
     <row r="41" ht="26" customHeight="1">
-      <c r="A41" s="37" t="inlineStr">
+      <c r="A41" s="36" t="inlineStr">
         <is>
           <t>SCALING_MAX_INSTANCES</t>
         </is>
       </c>
-      <c r="B41" s="38" t="inlineStr">
+      <c r="B41" s="37" t="inlineStr">
         <is>
           <t>Operations</t>
         </is>
       </c>
-      <c r="C41" s="39" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="D41" s="38" t="inlineStr">
+      <c r="C41" s="38" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="D41" s="37" t="inlineStr">
         <is>
           <t>10</t>
         </is>
       </c>
-      <c r="E41" s="38" t="inlineStr">
+      <c r="E41" s="37" t="inlineStr">
         <is>
           <t>Maximum number of instances</t>
         </is>
       </c>
-      <c r="F41" s="39" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G41" s="38" t="inlineStr">
+      <c r="F41" s="38" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G41" s="37" t="inlineStr">
         <is>
           <t>Integer</t>
         </is>
       </c>
-      <c r="H41" s="38" t="inlineStr">
+      <c r="H41" s="37" t="inlineStr">
         <is>
           <t>5-100</t>
         </is>
       </c>
-      <c r="I41" s="39" t="inlineStr">
+      <c r="I41" s="38" t="inlineStr">
         <is>
           <t>Public</t>
         </is>
       </c>
-      <c r="J41" s="38" t="inlineStr">
+      <c r="J41" s="37" t="inlineStr">
         <is>
           <t>Operations</t>
         </is>
       </c>
-      <c r="K41" s="38" t="inlineStr">
+      <c r="K41" s="37" t="inlineStr">
         <is>
           <t>Cost management</t>
         </is>
       </c>
-      <c r="L41" s="38" t="inlineStr">
+      <c r="L41" s="37" t="inlineStr">
         <is>
           <t>Set based on peak load</t>
         </is>
       </c>
-      <c r="M41" s="39" t="inlineStr">
+      <c r="M41" s="38" t="inlineStr">
         <is>
           <t>[DATE]</t>
         </is>
       </c>
     </row>
     <row r="42" ht="26" customHeight="1">
-      <c r="A42" s="40" t="inlineStr">
+      <c r="A42" s="39" t="inlineStr">
         <is>
           <t>SCALING_TARGET_CPU</t>
         </is>
       </c>
-      <c r="B42" s="41" t="inlineStr">
+      <c r="B42" s="40" t="inlineStr">
         <is>
           <t>Operations</t>
         </is>
       </c>
-      <c r="C42" s="42" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="D42" s="41" t="inlineStr">
+      <c r="C42" s="41" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="D42" s="40" t="inlineStr">
         <is>
           <t>70</t>
         </is>
       </c>
-      <c r="E42" s="41" t="inlineStr">
+      <c r="E42" s="40" t="inlineStr">
         <is>
           <t>CPU threshold for auto-scaling</t>
         </is>
       </c>
-      <c r="F42" s="42" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G42" s="41" t="inlineStr">
+      <c r="F42" s="41" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G42" s="40" t="inlineStr">
         <is>
           <t>Integer</t>
         </is>
       </c>
-      <c r="H42" s="41" t="inlineStr">
+      <c r="H42" s="40" t="inlineStr">
         <is>
           <t>50-90</t>
         </is>
       </c>
-      <c r="I42" s="42" t="inlineStr">
+      <c r="I42" s="41" t="inlineStr">
         <is>
           <t>Public</t>
         </is>
       </c>
-      <c r="J42" s="41" t="inlineStr">
+      <c r="J42" s="40" t="inlineStr">
         <is>
           <t>Operations</t>
         </is>
       </c>
-      <c r="K42" s="41" t="inlineStr">
+      <c r="K42" s="40" t="inlineStr">
         <is>
           <t>Performance monitoring</t>
         </is>
       </c>
-      <c r="L42" s="41" t="inlineStr">
+      <c r="L42" s="40" t="inlineStr">
         <is>
           <t>Tune based on application behavior</t>
         </is>
       </c>
-      <c r="M42" s="42" t="inlineStr">
+      <c r="M42" s="41" t="inlineStr">
         <is>
           <t>[DATE]</t>
         </is>

</xml_diff>